<commit_message>
added dark current plotter and some commenting
</commit_message>
<xml_diff>
--- a/analysis_page_darkCurrent.xlsx
+++ b/analysis_page_darkCurrent.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="27760" windowHeight="16900" xr2:uid="{1380874E-94DD-DB43-831B-EAA6682829BF}"/>
+    <workbookView xWindow="16080" yWindow="460" windowWidth="12720" windowHeight="16900" xr2:uid="{1380874E-94DD-DB43-831B-EAA6682829BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+  <si>
+    <t>Voltage (kV)</t>
+  </si>
+  <si>
+    <t>Run 0</t>
+  </si>
+  <si>
+    <t>Irradiated</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Filtered Average (pA)</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Filtered Average</t>
+  </si>
+  <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Run 3</t>
+  </si>
+  <si>
+    <t>Run 4</t>
+  </si>
+  <si>
+    <t>Timing</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="dd/mm/yy\ h:mm:ss"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -47,6 +87,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -70,10 +122,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,45 +445,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08157898-23EE-3741-B1EB-A1C0CD9DDBD8}">
-  <dimension ref="A3:AW122"/>
+  <dimension ref="A1:BE122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4:AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" customWidth="1"/>
+    <col min="22" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>17.02</v>
+      </c>
+      <c r="C4" s="5">
+        <v>42993.573854166665</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.7416666666666667</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="J4" s="5">
+        <v>43083.634456018517</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="M4" s="7">
+        <v>43083.395949074074</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1">
+        <v>2</v>
+      </c>
+      <c r="P4" s="1">
+        <v>-1.86</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>43174.688148148147</v>
+      </c>
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>8.74</v>
+      </c>
+      <c r="T4" s="5">
+        <v>43174.506724537037</v>
+      </c>
       <c r="U4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="V4" s="1">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="X4" s="5">
+        <v>43230.653773148151</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>43230.47896990741</v>
+      </c>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AE4" s="1"/>
+      <c r="AD4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AI4" s="1"/>
@@ -441,30 +706,90 @@
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="1"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35.89</v>
+      </c>
+      <c r="C5" s="5">
+        <v>42993.592048611114</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="J5" s="5">
+        <v>43083.640416666669</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="M5" s="7">
+        <v>43083.442118055558</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1">
+        <v>3</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>43174.683171296296</v>
+      </c>
+      <c r="R5" s="1">
+        <v>3</v>
+      </c>
+      <c r="S5" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>43174.501203703701</v>
+      </c>
       <c r="U5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="AA5" s="1"/>
+      <c r="V5" s="1">
+        <v>3</v>
+      </c>
+      <c r="W5" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="X5" s="5">
+        <v>43230.660682870373</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>43230.495162037034</v>
+      </c>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
@@ -480,30 +805,90 @@
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>55.9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42993.599351851852</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.76250000000000007</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>124.54</v>
+      </c>
+      <c r="J6" s="5">
+        <v>43083.657905092594</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M6" s="7">
+        <v>43083.453796296293</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>43174.678310185183</v>
+      </c>
+      <c r="R6" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="S6" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="T6" s="5">
+        <v>43174.494664351849</v>
+      </c>
       <c r="U6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="V6" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="W6" s="1">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="X6" s="5">
+        <v>43230.68922453704</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>29.94</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>43230.503344907411</v>
+      </c>
       <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
@@ -519,30 +904,90 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>96.4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>42993.657314814816</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.7715277777777777</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>308.23</v>
+      </c>
+      <c r="J7" s="5">
+        <v>43083.670706018522</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>11.77</v>
+      </c>
+      <c r="M7" s="7">
+        <v>43083.45789351852</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="P7" s="1">
+        <v>15.17</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>43174.673680555556</v>
+      </c>
+      <c r="R7" s="1">
+        <v>4</v>
+      </c>
+      <c r="S7" s="1">
+        <v>174</v>
+      </c>
+      <c r="T7" s="5">
+        <v>43174.489374999997</v>
+      </c>
       <c r="U7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="AA7" s="1"/>
+      <c r="V7" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>186.4</v>
+      </c>
+      <c r="X7" s="5">
+        <v>43230.69798611111</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>138.33000000000001</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>43230.521261574075</v>
+      </c>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
@@ -558,30 +1003,71 @@
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
+      <c r="BE7" s="1"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>145.72999999999999</v>
+      </c>
+      <c r="C8" s="5">
+        <v>42993.669791666667</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.77986111111111101</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="L8" s="1">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="M8" s="7">
+        <v>43083.462708333333</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="P8" s="1">
+        <v>23.48</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>43174.668715277781</v>
+      </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
+      <c r="V8" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="W8" s="1">
+        <v>190.7</v>
+      </c>
+      <c r="X8" s="5">
+        <v>43230.703969907408</v>
+      </c>
       <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
@@ -597,30 +1083,71 @@
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>217.19</v>
+      </c>
+      <c r="C9" s="5">
+        <v>42993.674178240741</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>40.9</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.78472222222222221</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="L9" s="1">
+        <v>21.83</v>
+      </c>
+      <c r="M9" s="7">
+        <v>43083.467418981483</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="P9" s="1">
+        <v>35.81</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>43174.662488425929</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
+      <c r="V9" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="W9" s="1">
+        <v>177</v>
+      </c>
+      <c r="X9" s="5">
+        <v>43230.718402777777</v>
+      </c>
       <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
@@ -636,30 +1163,71 @@
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
-    </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+    </row>
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>297.69</v>
+      </c>
+      <c r="C10" s="5">
+        <v>42993.678460648145</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.7909722222222223</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="L10" s="1">
+        <v>33.74</v>
+      </c>
+      <c r="M10" s="7">
+        <v>43083.471956018519</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="P10" s="1">
+        <v>64.47</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>43174.657222222224</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
+      <c r="V10" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="W10" s="1">
+        <v>223.4</v>
+      </c>
+      <c r="X10" s="5">
+        <v>43230.721458333333</v>
+      </c>
       <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
@@ -675,30 +1243,71 @@
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+    </row>
+    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>388.71</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42993.68787037037</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>136</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.7944444444444444</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="L11" s="1">
+        <v>53.52</v>
+      </c>
+      <c r="M11" s="7">
+        <v>43083.476493055554</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1">
+        <v>4</v>
+      </c>
+      <c r="P11" s="1">
+        <v>197.41</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>43174.651018518518</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
+      <c r="V11" s="1">
+        <v>4</v>
+      </c>
+      <c r="W11" s="1">
+        <v>425.3</v>
+      </c>
+      <c r="X11" s="5">
+        <v>43230.7266087963</v>
+      </c>
       <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
@@ -714,30 +1323,57 @@
       <c r="AU11" s="1"/>
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+    </row>
+    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>464.29</v>
+      </c>
+      <c r="C12" s="5">
+        <v>42993.706736111111</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="E12" s="1">
+        <v>194</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.80069444444444438</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1">
+        <v>4</v>
+      </c>
+      <c r="L12" s="1">
+        <v>128.07</v>
+      </c>
+      <c r="M12" s="7">
+        <v>43083.481192129628</v>
+      </c>
+      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
+      <c r="V12" s="1"/>
       <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
@@ -753,30 +1389,49 @@
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
-    </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="1"/>
+    </row>
+    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>607.04</v>
+      </c>
+      <c r="C13" s="5">
+        <v>42993.715671296297</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>264</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.80486111111111114</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
+      <c r="V13" s="1"/>
       <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
@@ -792,30 +1447,42 @@
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
+      <c r="BE13" s="1"/>
+    </row>
+    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>410</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.81041666666666667</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+      <c r="R14" s="1"/>
       <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
@@ -831,30 +1498,36 @@
       <c r="AU14" s="1"/>
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+    </row>
+    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
       <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
@@ -870,30 +1543,33 @@
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+    </row>
+    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
       <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
@@ -909,203 +1585,208 @@
       <c r="AU16" s="1"/>
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
-    </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
       <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
       <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
       <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
       <c r="AM17" s="1"/>
-      <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
-      <c r="AR17" s="1"/>
       <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
-      <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
-    </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
       <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
       <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
       <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
-      <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
-      <c r="AR18" s="1"/>
       <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
-      <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
-    </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+    </row>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="R19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-      <c r="W19" s="1"/>
+      <c r="V19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
-      <c r="AA19" s="1"/>
+      <c r="Z19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AE19" s="1"/>
+      <c r="AD19" s="1"/>
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
-      <c r="AI19" s="1"/>
+      <c r="AH19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
-      <c r="AM19" s="1"/>
+      <c r="AL19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
-      <c r="AQ19" s="1"/>
+      <c r="AP19" s="1"/>
       <c r="AR19" s="1"/>
       <c r="AS19" s="1"/>
-      <c r="AU19" s="1"/>
+      <c r="AT19" s="1"/>
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
-    </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AX19" s="1"/>
+    </row>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="J20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="N20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="R20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="W20" s="1"/>
+      <c r="V20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-      <c r="AA20" s="1"/>
+      <c r="Z20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
-      <c r="AE20" s="1"/>
+      <c r="AD20" s="1"/>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
-      <c r="AI20" s="1"/>
+      <c r="AH20" s="1"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
-      <c r="AM20" s="1"/>
+      <c r="AL20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
-      <c r="AQ20" s="1"/>
+      <c r="AP20" s="1"/>
       <c r="AR20" s="1"/>
       <c r="AS20" s="1"/>
-      <c r="AU20" s="1"/>
+      <c r="AT20" s="1"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
-    </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AX20" s="1"/>
+    </row>
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="J21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="N21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="R21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="W21" s="1"/>
+      <c r="V21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
-      <c r="AA21" s="1"/>
+      <c r="Z21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
-      <c r="AE21" s="1"/>
+      <c r="AD21" s="1"/>
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
-      <c r="AI21" s="1"/>
+      <c r="AH21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
-      <c r="AM21" s="1"/>
+      <c r="AL21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
-      <c r="AQ21" s="1"/>
+      <c r="AP21" s="1"/>
       <c r="AR21" s="1"/>
       <c r="AS21" s="1"/>
-      <c r="AU21" s="1"/>
+      <c r="AT21" s="1"/>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
-    </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AX21" s="1"/>
+    </row>
+    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1144,7 +1825,7 @@
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1183,7 +1864,7 @@
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1222,7 +1903,7 @@
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1261,7 +1942,7 @@
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1300,7 +1981,7 @@
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1339,7 +2020,7 @@
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1378,7 +2059,7 @@
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>

</xml_diff>